<commit_message>
Added Minutes of Meeting
</commit_message>
<xml_diff>
--- a/MOM/Minutes of Meetings.xlsx
+++ b/MOM/Minutes of Meetings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\OneDrive\Desktop\Trinity\Semester 2\Artificial Intelligence\AI_Project\Algorithms\MOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d2aff352e2fa15a/Desktop/AI/A2/Assignment2/Algorithms/MOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B11F30F-872B-4F2D-A9C0-4071FFFEE7C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{0B11F30F-872B-4F2D-A9C0-4071FFFEE7C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{169C2B89-7B80-4E81-9EFC-17C56750EB23}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{03220D0D-9A02-4F22-9290-0B7F15B79FF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03220D0D-9A02-4F22-9290-0B7F15B79FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="MOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,30 @@
   </si>
   <si>
     <t>Points to be covered for report writing.</t>
+  </si>
+  <si>
+    <t>Related Works on References - Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis - Vivek/Salil/ Priyanka
+Research Papers -All 
+Report Writing - Salil/Sneha
+PPt - Priyanka to start with
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Finish Report Writing by 28th April
+3. Finish Presentation Slides by 28th April
+4. Recording and submission by 29th April. </t>
+  </si>
+  <si>
+    <t>Report Writing - In process</t>
+  </si>
+  <si>
+    <t>Presentation Slides - To start</t>
+  </si>
+  <si>
+    <t>Analysis  - In progress</t>
   </si>
 </sst>
 </file>
@@ -503,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -532,6 +556,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,6 +590,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -550,14 +622,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -585,45 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,26 +966,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C67590E-0912-486D-8721-7324081545B2}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -978,131 +1005,131 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="22">
         <v>44288</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="36">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="18"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="18"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18">
+      <c r="D6" s="34"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="34">
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="18"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24"/>
       <c r="B12" s="6">
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="35"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1110,8 +1137,8 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+    <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
         <v>44291</v>
       </c>
       <c r="B14" s="9">
@@ -1120,73 +1147,73 @@
       <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="27"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18">
+      <c r="D15" s="34"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="34">
         <v>3</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="27"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="18"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="41"/>
+    </row>
+    <row r="19" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="28"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="D19" s="35"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
         <v>44296</v>
       </c>
       <c r="B21" s="9">
@@ -1195,150 +1222,150 @@
       <c r="C21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
       <c r="B22" s="1">
         <v>2</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18">
+      <c r="D22" s="34"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="34">
         <v>3</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="18"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="D26" s="35"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="22">
         <v>44302</v>
       </c>
-      <c r="B28" s="36">
+      <c r="B28" s="16">
         <v>1</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="37">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
+      <c r="B29" s="17">
         <v>2</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="38">
+      <c r="D29" s="34"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="23"/>
+      <c r="B30" s="31">
         <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="39"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="23"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="40"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="23"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="41">
+      <c r="D32" s="34"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="24"/>
+      <c r="B33" s="18">
         <v>4</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+      <c r="D33" s="35"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
         <v>44311</v>
       </c>
       <c r="B35" s="9">
@@ -1347,86 +1374,155 @@
       <c r="C35" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
       <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="43"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
       <c r="B37" s="13">
         <v>3</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="23"/>
       <c r="B38" s="13">
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="43"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
       <c r="B39" s="13">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="43"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="35"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="22"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="22">
+        <v>44313</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="23"/>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="26"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="20"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="14">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="20"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="23"/>
+      <c r="B45" s="14">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="23"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="24"/>
+      <c r="B47" s="15"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="F28:F33"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="F35:F40"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="E28:E33"/>
+  <mergeCells count="29">
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="A14:A19"/>
     <mergeCell ref="F21:F26"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="F2:F12"/>
@@ -1435,11 +1531,18 @@
     <mergeCell ref="F14:F19"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="E14:E19"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="F28:F33"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="B30:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>